<commit_message>
enh timeline and close the wbs in UI
</commit_message>
<xml_diff>
--- a/!important/docs/nephi networking.xlsx
+++ b/!important/docs/nephi networking.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabayon\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\nephi-networking\!important\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8616"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="WBS" sheetId="9" r:id="rId1"/>
     <sheet name="Risk" sheetId="5" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -808,7 +808,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1761,7 +1761,109 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1769,12 +1871,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1787,105 +1883,21 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1963,18 +1975,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2267,119 +2267,119 @@
   <dimension ref="A1:K66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K57" sqref="K57"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="52" customWidth="1"/>
-    <col min="4" max="4" width="3.88671875" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.44140625" style="25" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" customWidth="1"/>
-    <col min="9" max="9" width="11.5546875" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" customWidth="1"/>
-    <col min="11" max="11" width="18.109375" style="43" customWidth="1"/>
+    <col min="4" max="4" width="3.85546875" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.42578125" style="25" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" style="43" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="109" t="s">
+    <row r="1" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="111"/>
-      <c r="D1" s="111"/>
-      <c r="E1" s="111"/>
-      <c r="F1" s="112"/>
-      <c r="G1" s="112"/>
-      <c r="H1" s="112"/>
-      <c r="I1" s="112"/>
-      <c r="J1" s="112"/>
-      <c r="K1" s="113"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B1" s="90"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="92"/>
+      <c r="J1" s="92"/>
+      <c r="K1" s="93"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="10"/>
-      <c r="C2" s="118" t="s">
+      <c r="C2" s="100" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="119"/>
-      <c r="E2" s="119"/>
-      <c r="F2" s="119"/>
-      <c r="G2" s="120"/>
-      <c r="H2" s="116" t="s">
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="102"/>
+      <c r="H2" s="96" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="117"/>
-      <c r="J2" s="124" t="s">
+      <c r="I2" s="97"/>
+      <c r="J2" s="106" t="s">
         <v>57</v>
       </c>
-      <c r="K2" s="125"/>
-    </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K2" s="107"/>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="11"/>
-      <c r="C3" s="121" t="s">
+      <c r="C3" s="103" t="s">
         <v>59</v>
       </c>
-      <c r="D3" s="122"/>
-      <c r="E3" s="122"/>
-      <c r="F3" s="122"/>
-      <c r="G3" s="123"/>
-      <c r="H3" s="105" t="s">
+      <c r="D3" s="104"/>
+      <c r="E3" s="104"/>
+      <c r="F3" s="104"/>
+      <c r="G3" s="105"/>
+      <c r="H3" s="98" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="106"/>
-      <c r="J3" s="98">
+      <c r="I3" s="99"/>
+      <c r="J3" s="108">
         <v>43466</v>
       </c>
-      <c r="K3" s="99"/>
-    </row>
-    <row r="4" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K3" s="109"/>
+    </row>
+    <row r="4" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="11"/>
-      <c r="C4" s="102" t="s">
+      <c r="C4" s="112" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="103"/>
-      <c r="E4" s="103"/>
-      <c r="F4" s="103"/>
-      <c r="G4" s="104"/>
-      <c r="H4" s="105"/>
-      <c r="I4" s="106"/>
-      <c r="J4" s="98"/>
-      <c r="K4" s="99"/>
-    </row>
-    <row r="5" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="114"/>
-      <c r="B5" s="114"/>
-      <c r="C5" s="114"/>
-      <c r="D5" s="114"/>
-      <c r="E5" s="114"/>
-      <c r="F5" s="114"/>
-      <c r="G5" s="114"/>
-      <c r="H5" s="114"/>
-      <c r="I5" s="114"/>
-      <c r="J5" s="114"/>
-      <c r="K5" s="114"/>
-    </row>
-    <row r="6" spans="1:11" s="19" customFormat="1" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D4" s="113"/>
+      <c r="E4" s="113"/>
+      <c r="F4" s="113"/>
+      <c r="G4" s="114"/>
+      <c r="H4" s="98"/>
+      <c r="I4" s="99"/>
+      <c r="J4" s="108"/>
+      <c r="K4" s="109"/>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="94"/>
+      <c r="B5" s="94"/>
+      <c r="C5" s="94"/>
+      <c r="D5" s="94"/>
+      <c r="E5" s="94"/>
+      <c r="F5" s="94"/>
+      <c r="G5" s="94"/>
+      <c r="H5" s="94"/>
+      <c r="I5" s="94"/>
+      <c r="J5" s="94"/>
+      <c r="K5" s="94"/>
+    </row>
+    <row r="6" spans="1:11" s="19" customFormat="1" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="115" t="s">
+      <c r="B6" s="95" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="115"/>
+      <c r="C6" s="95"/>
       <c r="D6" s="23" t="s">
         <v>8</v>
       </c>
@@ -2405,15 +2405,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="64">
         <v>1</v>
       </c>
-      <c r="B7" s="107" t="str">
+      <c r="B7" s="115" t="str">
         <f>C2</f>
         <v>Zerhuel Bussiness Networking</v>
       </c>
-      <c r="C7" s="108"/>
+      <c r="C7" s="116"/>
       <c r="D7" s="46"/>
       <c r="E7" s="46"/>
       <c r="F7" s="66"/>
@@ -2423,14 +2423,14 @@
       <c r="J7" s="46"/>
       <c r="K7" s="58"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="44">
         <v>2</v>
       </c>
-      <c r="B8" s="89" t="s">
+      <c r="B8" s="85" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="90"/>
+      <c r="C8" s="86"/>
       <c r="D8" s="48"/>
       <c r="E8" s="48"/>
       <c r="F8" s="67"/>
@@ -2440,7 +2440,7 @@
       <c r="J8" s="48"/>
       <c r="K8" s="59"/>
     </row>
-    <row r="9" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="44">
         <v>3</v>
       </c>
@@ -2469,7 +2469,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="33" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" s="33" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="44">
         <v>4</v>
       </c>
@@ -2498,7 +2498,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="34">
         <v>5</v>
       </c>
@@ -2527,7 +2527,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="44">
         <v>8</v>
       </c>
@@ -2556,7 +2556,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="44"/>
       <c r="B13" s="83"/>
       <c r="C13" s="84"/>
@@ -2569,14 +2569,14 @@
       <c r="J13" s="35"/>
       <c r="K13" s="26"/>
     </row>
-    <row r="14" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="44">
         <v>9</v>
       </c>
-      <c r="B14" s="89" t="s">
+      <c r="B14" s="85" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="90"/>
+      <c r="C14" s="86"/>
       <c r="D14" s="48"/>
       <c r="E14" s="48"/>
       <c r="F14" s="67"/>
@@ -2586,7 +2586,7 @@
       <c r="J14" s="48"/>
       <c r="K14" s="59"/>
     </row>
-    <row r="15" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="44">
         <v>10</v>
       </c>
@@ -2615,7 +2615,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="44">
         <v>11</v>
       </c>
@@ -2644,14 +2644,14 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="44">
         <v>12</v>
       </c>
-      <c r="B17" s="100" t="s">
+      <c r="B17" s="110" t="s">
         <v>65</v>
       </c>
-      <c r="C17" s="101"/>
+      <c r="C17" s="111"/>
       <c r="D17" s="73"/>
       <c r="E17" s="35" t="s">
         <v>28</v>
@@ -2673,7 +2673,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="44">
         <v>13</v>
       </c>
@@ -2700,7 +2700,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="44">
         <v>14</v>
       </c>
@@ -2729,7 +2729,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="44">
         <v>15</v>
       </c>
@@ -2756,7 +2756,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="44">
         <v>16</v>
       </c>
@@ -2785,7 +2785,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="44">
         <v>17</v>
       </c>
@@ -2814,7 +2814,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="44">
         <v>18</v>
       </c>
@@ -2841,7 +2841,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="44">
         <v>19</v>
       </c>
@@ -2870,7 +2870,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="44"/>
       <c r="B25" s="83"/>
       <c r="C25" s="84"/>
@@ -2883,10 +2883,10 @@
       <c r="J25" s="35"/>
       <c r="K25" s="26"/>
     </row>
-    <row r="26" spans="1:11" s="33" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" s="33" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="44"/>
-      <c r="B26" s="95"/>
-      <c r="C26" s="96"/>
+      <c r="B26" s="118"/>
+      <c r="C26" s="119"/>
       <c r="D26" s="37"/>
       <c r="E26" s="35"/>
       <c r="F26" s="68"/>
@@ -2896,14 +2896,14 @@
       <c r="J26" s="37"/>
       <c r="K26" s="26"/>
     </row>
-    <row r="27" spans="1:11" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="34">
         <v>21</v>
       </c>
-      <c r="B27" s="89" t="s">
+      <c r="B27" s="85" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="90"/>
+      <c r="C27" s="86"/>
       <c r="D27" s="52"/>
       <c r="E27" s="52"/>
       <c r="F27" s="70"/>
@@ -2913,7 +2913,7 @@
       <c r="J27" s="52"/>
       <c r="K27" s="61"/>
     </row>
-    <row r="28" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="44">
         <v>22</v>
       </c>
@@ -2923,7 +2923,7 @@
       <c r="C28" s="84"/>
       <c r="D28" s="35"/>
       <c r="E28" s="35" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F28" s="68">
         <v>8</v>
@@ -2940,7 +2940,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="34">
         <v>23</v>
       </c>
@@ -2967,7 +2967,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="44">
         <v>24</v>
       </c>
@@ -2994,7 +2994,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="34">
         <v>25</v>
       </c>
@@ -3021,7 +3021,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="44">
         <v>26</v>
       </c>
@@ -3048,7 +3048,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="34">
         <v>27</v>
       </c>
@@ -3075,7 +3075,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="34"/>
       <c r="B34" s="83" t="s">
         <v>76</v>
@@ -3100,7 +3100,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="34"/>
       <c r="B35" s="83" t="s">
         <v>78</v>
@@ -3125,7 +3125,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="34"/>
       <c r="B36" s="83" t="s">
         <v>79</v>
@@ -3150,7 +3150,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="34"/>
       <c r="B37" s="83" t="s">
         <v>80</v>
@@ -3175,7 +3175,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="34"/>
       <c r="B38" s="83" t="s">
         <v>81</v>
@@ -3200,7 +3200,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="34"/>
       <c r="B39" s="83" t="s">
         <v>84</v>
@@ -3225,7 +3225,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="34"/>
       <c r="B40" s="83" t="s">
         <v>82</v>
@@ -3250,7 +3250,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="34"/>
       <c r="B41" s="83" t="s">
         <v>83</v>
@@ -3275,7 +3275,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="34"/>
       <c r="B42" s="83" t="s">
         <v>85</v>
@@ -3300,10 +3300,10 @@
         <v>95</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="44"/>
-      <c r="B43" s="87"/>
-      <c r="C43" s="88"/>
+      <c r="B43" s="121"/>
+      <c r="C43" s="122"/>
       <c r="D43" s="35"/>
       <c r="E43" s="35"/>
       <c r="F43" s="68"/>
@@ -3313,14 +3313,14 @@
       <c r="J43" s="35"/>
       <c r="K43" s="26"/>
     </row>
-    <row r="44" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="44">
         <v>28</v>
       </c>
-      <c r="B44" s="89" t="s">
+      <c r="B44" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="C44" s="90"/>
+      <c r="C44" s="86"/>
       <c r="D44" s="48"/>
       <c r="E44" s="48"/>
       <c r="F44" s="67"/>
@@ -3330,7 +3330,7 @@
       <c r="J44" s="48"/>
       <c r="K44" s="59"/>
     </row>
-    <row r="45" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="44">
         <v>29</v>
       </c>
@@ -3357,7 +3357,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="44">
         <v>30</v>
       </c>
@@ -3384,7 +3384,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="44"/>
       <c r="B47" s="83"/>
       <c r="C47" s="84"/>
@@ -3397,14 +3397,14 @@
       <c r="J47" s="35"/>
       <c r="K47" s="26"/>
     </row>
-    <row r="48" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="44">
         <v>31</v>
       </c>
-      <c r="B48" s="89" t="s">
+      <c r="B48" s="85" t="s">
         <v>21</v>
       </c>
-      <c r="C48" s="90"/>
+      <c r="C48" s="86"/>
       <c r="D48" s="48"/>
       <c r="E48" s="48"/>
       <c r="F48" s="67"/>
@@ -3414,7 +3414,7 @@
       <c r="J48" s="48"/>
       <c r="K48" s="59"/>
     </row>
-    <row r="49" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="44">
         <v>32</v>
       </c>
@@ -3441,7 +3441,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="29"/>
       <c r="B50" s="83"/>
       <c r="C50" s="84"/>
@@ -3454,14 +3454,14 @@
       <c r="J50" s="41"/>
       <c r="K50" s="62"/>
     </row>
-    <row r="51" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="44">
         <v>33</v>
       </c>
-      <c r="B51" s="89" t="s">
+      <c r="B51" s="85" t="s">
         <v>22</v>
       </c>
-      <c r="C51" s="90"/>
+      <c r="C51" s="86"/>
       <c r="D51" s="48"/>
       <c r="E51" s="48"/>
       <c r="F51" s="67"/>
@@ -3471,7 +3471,7 @@
       <c r="J51" s="48"/>
       <c r="K51" s="59"/>
     </row>
-    <row r="52" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="44">
         <v>34</v>
       </c>
@@ -3498,7 +3498,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="44">
         <v>35</v>
       </c>
@@ -3527,7 +3527,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="44"/>
       <c r="B54" s="83"/>
       <c r="C54" s="84"/>
@@ -3539,12 +3539,12 @@
       <c r="J54" s="35"/>
       <c r="K54" s="26"/>
     </row>
-    <row r="55" spans="1:11" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:11" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="65"/>
-      <c r="B55" s="126" t="s">
+      <c r="B55" s="87" t="s">
         <v>24</v>
       </c>
-      <c r="C55" s="127"/>
+      <c r="C55" s="88"/>
       <c r="D55" s="55"/>
       <c r="E55" s="55"/>
       <c r="F55" s="72"/>
@@ -3554,12 +3554,12 @@
       <c r="J55" s="55"/>
       <c r="K55" s="63"/>
     </row>
-    <row r="56" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="57" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B57" s="93" t="s">
+    <row r="56" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="57" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="125" t="s">
         <v>25</v>
       </c>
-      <c r="C57" s="94"/>
+      <c r="C57" s="126"/>
       <c r="D57" s="78"/>
       <c r="E57" s="78"/>
       <c r="F57" s="78" t="s">
@@ -3572,8 +3572,8 @@
       </c>
       <c r="K57"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B58" s="91" t="s">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B58" s="123" t="s">
         <v>9</v>
       </c>
       <c r="C58" s="76" t="s">
@@ -3587,8 +3587,8 @@
       <c r="I58" s="81"/>
       <c r="K58"/>
     </row>
-    <row r="59" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B59" s="92"/>
+    <row r="59" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="124"/>
       <c r="C59" s="77" t="s">
         <v>29</v>
       </c>
@@ -3600,7 +3600,7 @@
       <c r="I59" s="81"/>
       <c r="K59"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B60" s="78"/>
       <c r="C60" s="78"/>
       <c r="D60" s="78"/>
@@ -3615,7 +3615,7 @@
       </c>
       <c r="K60"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B61" s="78"/>
       <c r="C61" s="78"/>
       <c r="D61" s="78"/>
@@ -3630,84 +3630,64 @@
       </c>
       <c r="K61"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B62" s="78"/>
       <c r="C62" s="78"/>
       <c r="D62" s="78"/>
       <c r="E62" s="78"/>
-      <c r="F62" s="85"/>
-      <c r="G62" s="85"/>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F62" s="117"/>
+      <c r="G62" s="117"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B63" s="78"/>
       <c r="C63" s="78"/>
       <c r="D63" s="78"/>
       <c r="E63" s="78"/>
-      <c r="F63" s="85"/>
-      <c r="G63" s="85"/>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F63" s="117"/>
+      <c r="G63" s="117"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B64" s="78"/>
       <c r="C64" s="78"/>
       <c r="D64" s="78"/>
       <c r="E64" s="78"/>
-      <c r="F64" s="85"/>
-      <c r="G64" s="85"/>
-    </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F64" s="117"/>
+      <c r="G64" s="117"/>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B65" s="78"/>
       <c r="C65" s="79"/>
       <c r="D65" s="78"/>
       <c r="E65" s="78"/>
-      <c r="F65" s="86"/>
-      <c r="G65" s="86"/>
-    </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F65" s="120"/>
+      <c r="G65" s="120"/>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B66" s="78"/>
       <c r="C66" s="78"/>
       <c r="D66" s="78"/>
       <c r="E66" s="78"/>
-      <c r="F66" s="85"/>
-      <c r="G66" s="85"/>
+      <c r="F66" s="117"/>
+      <c r="G66" s="117"/>
     </row>
   </sheetData>
   <mergeCells count="68">
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A5:K5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="C2:G2"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="F62:G62"/>
+    <mergeCell ref="F63:G63"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B49:C49"/>
     <mergeCell ref="F66:G66"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="B10:C10"/>
@@ -3724,22 +3704,42 @@
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="B31:C31"/>
-    <mergeCell ref="F62:G62"/>
-    <mergeCell ref="F63:G63"/>
-    <mergeCell ref="F64:G64"/>
-    <mergeCell ref="F65:G65"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A5:K5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7:E8 E14 E27 E44 E48 E51 E55">
@@ -3760,109 +3760,109 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.33203125" style="25" customWidth="1"/>
-    <col min="2" max="2" width="37.44140625" customWidth="1"/>
-    <col min="3" max="5" width="3.6640625" customWidth="1"/>
-    <col min="6" max="6" width="3.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" customWidth="1"/>
-    <col min="8" max="8" width="21.88671875" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" style="25" customWidth="1"/>
+    <col min="2" max="2" width="37.42578125" customWidth="1"/>
+    <col min="3" max="5" width="3.7109375" customWidth="1"/>
+    <col min="6" max="6" width="3.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" customWidth="1"/>
+    <col min="8" max="8" width="21.85546875" customWidth="1"/>
     <col min="9" max="9" width="20" customWidth="1"/>
-    <col min="10" max="10" width="31.44140625" customWidth="1"/>
+    <col min="10" max="10" width="31.42578125" customWidth="1"/>
     <col min="11" max="11" width="21" customWidth="1"/>
-    <col min="12" max="12" width="9.44140625" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" customWidth="1"/>
     <col min="13" max="13" width="7" customWidth="1"/>
-    <col min="14" max="15" width="8.5546875" customWidth="1"/>
+    <col min="14" max="15" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="109" t="s">
+    <row r="1" spans="1:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="89" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="111"/>
-      <c r="D1" s="111"/>
-      <c r="E1" s="111"/>
-      <c r="F1" s="111"/>
-      <c r="G1" s="111"/>
-      <c r="H1" s="111"/>
-      <c r="I1" s="111"/>
-      <c r="J1" s="111"/>
-      <c r="K1" s="111"/>
-      <c r="L1" s="112"/>
-      <c r="M1" s="112"/>
-      <c r="N1" s="112"/>
-      <c r="O1" s="113"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="154" t="s">
+      <c r="B1" s="90"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="91"/>
+      <c r="I1" s="91"/>
+      <c r="J1" s="91"/>
+      <c r="K1" s="91"/>
+      <c r="L1" s="92"/>
+      <c r="M1" s="92"/>
+      <c r="N1" s="92"/>
+      <c r="O1" s="93"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="127" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="155"/>
-      <c r="C2" s="118" t="s">
+      <c r="B2" s="128"/>
+      <c r="C2" s="100" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="119"/>
-      <c r="E2" s="119"/>
-      <c r="F2" s="119"/>
-      <c r="G2" s="119"/>
-      <c r="H2" s="120"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="102"/>
       <c r="I2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="124" t="s">
+      <c r="J2" s="106" t="s">
         <v>57</v>
       </c>
-      <c r="K2" s="125"/>
-      <c r="L2" s="124"/>
-      <c r="M2" s="125"/>
-      <c r="N2" s="124"/>
-      <c r="O2" s="125"/>
-    </row>
-    <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="156" t="s">
+      <c r="K2" s="107"/>
+      <c r="L2" s="106"/>
+      <c r="M2" s="107"/>
+      <c r="N2" s="106"/>
+      <c r="O2" s="107"/>
+    </row>
+    <row r="3" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="129" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="157"/>
-      <c r="C3" s="121" t="s">
+      <c r="B3" s="130"/>
+      <c r="C3" s="103" t="s">
         <v>94</v>
       </c>
-      <c r="D3" s="122"/>
-      <c r="E3" s="122"/>
-      <c r="F3" s="122"/>
-      <c r="G3" s="122"/>
-      <c r="H3" s="123"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="104"/>
+      <c r="F3" s="104"/>
+      <c r="G3" s="104"/>
+      <c r="H3" s="105"/>
       <c r="I3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="97">
+      <c r="J3" s="131">
         <v>43466</v>
       </c>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
-      <c r="O3" s="99"/>
-    </row>
-    <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="114"/>
-      <c r="B4" s="114"/>
-      <c r="C4" s="114"/>
-      <c r="D4" s="114"/>
-      <c r="E4" s="114"/>
-      <c r="F4" s="114"/>
-      <c r="G4" s="114"/>
-      <c r="H4" s="114"/>
-      <c r="I4" s="114"/>
-      <c r="J4" s="114"/>
-      <c r="K4" s="114"/>
-      <c r="L4" s="114"/>
-      <c r="M4" s="114"/>
-      <c r="N4" s="114"/>
-      <c r="O4" s="114"/>
-    </row>
-    <row r="5" spans="1:15" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="K3" s="108"/>
+      <c r="L3" s="108"/>
+      <c r="M3" s="108"/>
+      <c r="N3" s="108"/>
+      <c r="O3" s="109"/>
+    </row>
+    <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="94"/>
+      <c r="B4" s="94"/>
+      <c r="C4" s="94"/>
+      <c r="D4" s="94"/>
+      <c r="E4" s="94"/>
+      <c r="F4" s="94"/>
+      <c r="G4" s="94"/>
+      <c r="H4" s="94"/>
+      <c r="I4" s="94"/>
+      <c r="J4" s="94"/>
+      <c r="K4" s="94"/>
+      <c r="L4" s="94"/>
+      <c r="M4" s="94"/>
+      <c r="N4" s="94"/>
+      <c r="O4" s="94"/>
+    </row>
+    <row r="5" spans="1:15" ht="65.25" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
         <v>6</v>
       </c>
@@ -3909,7 +3909,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="44">
         <v>2</v>
       </c>
@@ -3931,7 +3931,7 @@
       <c r="N6" s="3"/>
       <c r="O6" s="4"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="44">
         <v>3</v>
       </c>
@@ -3953,7 +3953,7 @@
       <c r="N7" s="3"/>
       <c r="O7" s="4"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="44">
         <v>4</v>
       </c>
@@ -3975,7 +3975,7 @@
       <c r="N8" s="3"/>
       <c r="O8" s="4"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="44">
         <v>5</v>
       </c>
@@ -3997,7 +3997,7 @@
       <c r="N9" s="3"/>
       <c r="O9" s="4"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="44">
         <v>6</v>
       </c>
@@ -4019,7 +4019,7 @@
       <c r="N10" s="3"/>
       <c r="O10" s="4"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="44">
         <v>7</v>
       </c>
@@ -4041,7 +4041,7 @@
       <c r="N11" s="3"/>
       <c r="O11" s="4"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="44">
         <v>8</v>
       </c>
@@ -4063,7 +4063,7 @@
       <c r="N12" s="3"/>
       <c r="O12" s="4"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="44">
         <v>9</v>
       </c>
@@ -4085,7 +4085,7 @@
       <c r="N13" s="3"/>
       <c r="O13" s="4"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="44">
         <v>10</v>
       </c>
@@ -4107,7 +4107,7 @@
       <c r="N14" s="3"/>
       <c r="O14" s="4"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="44">
         <v>11</v>
       </c>
@@ -4129,7 +4129,7 @@
       <c r="N15" s="3"/>
       <c r="O15" s="4"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="44">
         <v>12</v>
       </c>
@@ -4151,7 +4151,7 @@
       <c r="N16" s="3"/>
       <c r="O16" s="4"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="44">
         <v>13</v>
       </c>
@@ -4173,7 +4173,7 @@
       <c r="N17" s="3"/>
       <c r="O17" s="4"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="44">
         <v>14</v>
       </c>
@@ -4195,7 +4195,7 @@
       <c r="N18" s="3"/>
       <c r="O18" s="4"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="44">
         <v>15</v>
       </c>
@@ -4217,7 +4217,7 @@
       <c r="N19" s="3"/>
       <c r="O19" s="4"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="44">
         <v>16</v>
       </c>
@@ -4239,7 +4239,7 @@
       <c r="N20" s="3"/>
       <c r="O20" s="4"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="44">
         <v>17</v>
       </c>
@@ -4261,7 +4261,7 @@
       <c r="N21" s="3"/>
       <c r="O21" s="4"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="44">
         <v>18</v>
       </c>
@@ -4283,7 +4283,7 @@
       <c r="N22" s="3"/>
       <c r="O22" s="4"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="44">
         <v>19</v>
       </c>
@@ -4305,7 +4305,7 @@
       <c r="N23" s="3"/>
       <c r="O23" s="4"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="44">
         <v>20</v>
       </c>
@@ -4327,7 +4327,7 @@
       <c r="N24" s="3"/>
       <c r="O24" s="4"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="44">
         <v>21</v>
       </c>
@@ -4349,7 +4349,7 @@
       <c r="N25" s="3"/>
       <c r="O25" s="4"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="44">
         <v>22</v>
       </c>
@@ -4371,7 +4371,7 @@
       <c r="N26" s="3"/>
       <c r="O26" s="4"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="44">
         <v>23</v>
       </c>
@@ -4393,7 +4393,7 @@
       <c r="N27" s="3"/>
       <c r="O27" s="4"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="44">
         <v>24</v>
       </c>
@@ -4415,7 +4415,7 @@
       <c r="N28" s="3"/>
       <c r="O28" s="4"/>
     </row>
-    <row r="29" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="24">
         <v>25</v>
       </c>
@@ -4437,131 +4437,122 @@
       <c r="N29" s="9"/>
       <c r="O29" s="5"/>
     </row>
-    <row r="31" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>46</v>
       </c>
       <c r="F31" s="43"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B32" s="134" t="s">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B32" s="138" t="s">
         <v>47</v>
       </c>
-      <c r="C32" s="137">
+      <c r="C32" s="141">
         <v>4</v>
       </c>
-      <c r="D32" s="138"/>
-      <c r="E32" s="138"/>
-      <c r="F32" s="139"/>
+      <c r="D32" s="142"/>
+      <c r="E32" s="142"/>
+      <c r="F32" s="143"/>
       <c r="G32" s="13"/>
       <c r="H32" s="13"/>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B33" s="135"/>
-      <c r="C33" s="140">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="139"/>
+      <c r="C33" s="144">
         <v>3</v>
       </c>
-      <c r="D33" s="141"/>
-      <c r="E33" s="141"/>
-      <c r="F33" s="142"/>
+      <c r="D33" s="145"/>
+      <c r="E33" s="145"/>
+      <c r="F33" s="146"/>
       <c r="G33" s="15"/>
       <c r="H33" s="15"/>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B34" s="135"/>
-      <c r="C34" s="140">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="139"/>
+      <c r="C34" s="144">
         <v>2</v>
       </c>
-      <c r="D34" s="141"/>
-      <c r="E34" s="141"/>
-      <c r="F34" s="142"/>
+      <c r="D34" s="145"/>
+      <c r="E34" s="145"/>
+      <c r="F34" s="146"/>
       <c r="G34" s="15"/>
       <c r="H34" s="15"/>
     </row>
-    <row r="35" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="136"/>
-      <c r="C35" s="143">
+    <row r="35" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="140"/>
+      <c r="C35" s="147">
         <v>1</v>
       </c>
-      <c r="D35" s="144"/>
-      <c r="E35" s="144"/>
-      <c r="F35" s="145"/>
+      <c r="D35" s="148"/>
+      <c r="E35" s="148"/>
+      <c r="F35" s="149"/>
       <c r="G35" s="15"/>
       <c r="H35" s="15"/>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B36" s="152" t="s">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="156" t="s">
         <v>38</v>
       </c>
-      <c r="C36" s="146" t="s">
+      <c r="C36" s="150" t="s">
         <v>48</v>
       </c>
-      <c r="D36" s="147"/>
-      <c r="E36" s="147"/>
-      <c r="F36" s="148"/>
+      <c r="D36" s="151"/>
+      <c r="E36" s="151"/>
+      <c r="F36" s="152"/>
       <c r="G36" s="15"/>
       <c r="H36" s="15"/>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B37" s="135"/>
-      <c r="C37" s="140" t="s">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="139"/>
+      <c r="C37" s="144" t="s">
         <v>49</v>
       </c>
-      <c r="D37" s="141"/>
-      <c r="E37" s="141"/>
-      <c r="F37" s="142"/>
+      <c r="D37" s="145"/>
+      <c r="E37" s="145"/>
+      <c r="F37" s="146"/>
       <c r="G37" s="14"/>
       <c r="H37" s="14"/>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B38" s="135"/>
-      <c r="C38" s="140" t="s">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="139"/>
+      <c r="C38" s="144" t="s">
         <v>44</v>
       </c>
-      <c r="D38" s="141"/>
-      <c r="E38" s="141"/>
-      <c r="F38" s="142"/>
-    </row>
-    <row r="39" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="153"/>
-      <c r="C39" s="149" t="s">
+      <c r="D38" s="145"/>
+      <c r="E38" s="145"/>
+      <c r="F38" s="146"/>
+    </row>
+    <row r="39" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="157"/>
+      <c r="C39" s="153" t="s">
         <v>45</v>
       </c>
-      <c r="D39" s="150"/>
-      <c r="E39" s="150"/>
-      <c r="F39" s="151"/>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B40" s="132" t="s">
+      <c r="D39" s="154"/>
+      <c r="E39" s="154"/>
+      <c r="F39" s="155"/>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="136" t="s">
         <v>9</v>
       </c>
-      <c r="C40" s="128" t="s">
+      <c r="C40" s="132" t="s">
         <v>28</v>
       </c>
-      <c r="D40" s="128"/>
-      <c r="E40" s="128"/>
-      <c r="F40" s="129"/>
-    </row>
-    <row r="41" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="133"/>
-      <c r="C41" s="130" t="s">
+      <c r="D40" s="132"/>
+      <c r="E40" s="132"/>
+      <c r="F40" s="133"/>
+    </row>
+    <row r="41" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="137"/>
+      <c r="C41" s="134" t="s">
         <v>29</v>
       </c>
-      <c r="D41" s="130"/>
-      <c r="E41" s="130"/>
-      <c r="F41" s="131"/>
+      <c r="D41" s="134"/>
+      <c r="E41" s="134"/>
+      <c r="F41" s="135"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="A4:O4"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="J3:O3"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="N2:O2"/>
     <mergeCell ref="C40:F40"/>
     <mergeCell ref="C41:F41"/>
     <mergeCell ref="B40:B41"/>
@@ -4576,6 +4567,15 @@
     <mergeCell ref="C38:F38"/>
     <mergeCell ref="C39:F39"/>
     <mergeCell ref="B36:B39"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A4:O4"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="J3:O3"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:O2"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14:E29">
@@ -4598,33 +4598,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Cost_x0020_Center xmlns="de1f3527-ee65-4171-8e88-278d1cad4dba" xsi:nil="true"/>
-    <SharedWithUsers xmlns="93e0a51c-8a94-4846-800d-92cf8a641c81">
-      <UserInfo>
-        <DisplayName>Mileesa Lumanog</DisplayName>
-        <AccountId>209</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Rosemarie Cris Flores</DisplayName>
-        <AccountId>207</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Malou Joy E. Bangcong</DisplayName>
-        <AccountId>273</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Leilah King</DisplayName>
-        <AccountId>208</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4836,21 +4815,39 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Cost_x0020_Center xmlns="de1f3527-ee65-4171-8e88-278d1cad4dba" xsi:nil="true"/>
+    <SharedWithUsers xmlns="93e0a51c-8a94-4846-800d-92cf8a641c81">
+      <UserInfo>
+        <DisplayName>Mileesa Lumanog</DisplayName>
+        <AccountId>209</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Rosemarie Cris Flores</DisplayName>
+        <AccountId>207</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Malou Joy E. Bangcong</DisplayName>
+        <AccountId>273</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Leilah King</DisplayName>
+        <AccountId>208</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36FA0B68-4ACD-45C2-9A26-792212BEB904}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{920A0596-903B-4E80-BD3E-00D8BD1A98DD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="de1f3527-ee65-4171-8e88-278d1cad4dba"/>
-    <ds:schemaRef ds:uri="93e0a51c-8a94-4846-800d-92cf8a641c81"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4876,9 +4873,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{920A0596-903B-4E80-BD3E-00D8BD1A98DD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36FA0B68-4ACD-45C2-9A26-792212BEB904}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="de1f3527-ee65-4171-8e88-278d1cad4dba"/>
+    <ds:schemaRef ds:uri="93e0a51c-8a94-4846-800d-92cf8a641c81"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add scarfonictech CI standard template
</commit_message>
<xml_diff>
--- a/!important/docs/nephi networking.xlsx
+++ b/!important/docs/nephi networking.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="WBS" sheetId="9" r:id="rId1"/>
     <sheet name="Risk" sheetId="5" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -512,7 +512,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="102">
   <si>
     <t>WORK BREAKDOWN STRUCTURE</t>
   </si>
@@ -803,12 +803,27 @@
   </si>
   <si>
     <t>Cocoy/Nephi</t>
+  </si>
+  <si>
+    <t>https://carlodimaandal.com/how-much-does-a-website-cost-in-the-philippines</t>
+  </si>
+  <si>
+    <t>https://www.freehostia.com/free-cloud-hosting/</t>
+  </si>
+  <si>
+    <t>https://www.digitalberg.com/free-ssd-web-hosting-cloud/</t>
+  </si>
+  <si>
+    <t>https://vpsie.com/pricing/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1755,133 +1770,211 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1897,84 +1990,6 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2266,120 +2281,120 @@
   </sheetPr>
   <dimension ref="A1:K66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9:F53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
     <col min="3" max="3" width="52" customWidth="1"/>
-    <col min="4" max="4" width="3.85546875" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.42578125" style="25" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" customWidth="1"/>
-    <col min="11" max="11" width="18.140625" style="43" customWidth="1"/>
+    <col min="4" max="4" width="3.88671875" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.44140625" style="25" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" customWidth="1"/>
+    <col min="9" max="9" width="11.5546875" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" customWidth="1"/>
+    <col min="11" max="11" width="18.109375" style="43" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="89" t="s">
+    <row r="1" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="108" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="92"/>
-      <c r="H1" s="92"/>
-      <c r="I1" s="92"/>
-      <c r="J1" s="92"/>
-      <c r="K1" s="93"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B1" s="109"/>
+      <c r="C1" s="110"/>
+      <c r="D1" s="110"/>
+      <c r="E1" s="110"/>
+      <c r="F1" s="111"/>
+      <c r="G1" s="111"/>
+      <c r="H1" s="111"/>
+      <c r="I1" s="111"/>
+      <c r="J1" s="111"/>
+      <c r="K1" s="112"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="10"/>
-      <c r="C2" s="100" t="s">
+      <c r="C2" s="117" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="101"/>
-      <c r="E2" s="101"/>
-      <c r="F2" s="101"/>
-      <c r="G2" s="102"/>
-      <c r="H2" s="96" t="s">
+      <c r="D2" s="118"/>
+      <c r="E2" s="118"/>
+      <c r="F2" s="118"/>
+      <c r="G2" s="119"/>
+      <c r="H2" s="115" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="97"/>
-      <c r="J2" s="106" t="s">
+      <c r="I2" s="116"/>
+      <c r="J2" s="123" t="s">
         <v>57</v>
       </c>
-      <c r="K2" s="107"/>
-    </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K2" s="124"/>
+    </row>
+    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="11"/>
-      <c r="C3" s="103" t="s">
+      <c r="C3" s="120" t="s">
         <v>59</v>
       </c>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="105"/>
-      <c r="H3" s="98" t="s">
+      <c r="D3" s="121"/>
+      <c r="E3" s="121"/>
+      <c r="F3" s="121"/>
+      <c r="G3" s="122"/>
+      <c r="H3" s="104" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="99"/>
-      <c r="J3" s="108">
+      <c r="I3" s="105"/>
+      <c r="J3" s="97">
         <v>43466</v>
       </c>
-      <c r="K3" s="109"/>
-    </row>
-    <row r="4" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K3" s="98"/>
+    </row>
+    <row r="4" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="11"/>
-      <c r="C4" s="112" t="s">
+      <c r="C4" s="101" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="113"/>
-      <c r="E4" s="113"/>
-      <c r="F4" s="113"/>
-      <c r="G4" s="114"/>
-      <c r="H4" s="98"/>
-      <c r="I4" s="99"/>
-      <c r="J4" s="108"/>
-      <c r="K4" s="109"/>
-    </row>
-    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="94"/>
-      <c r="B5" s="94"/>
-      <c r="C5" s="94"/>
-      <c r="D5" s="94"/>
-      <c r="E5" s="94"/>
-      <c r="F5" s="94"/>
-      <c r="G5" s="94"/>
-      <c r="H5" s="94"/>
-      <c r="I5" s="94"/>
-      <c r="J5" s="94"/>
-      <c r="K5" s="94"/>
-    </row>
-    <row r="6" spans="1:11" s="19" customFormat="1" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="102"/>
+      <c r="E4" s="102"/>
+      <c r="F4" s="102"/>
+      <c r="G4" s="103"/>
+      <c r="H4" s="104"/>
+      <c r="I4" s="105"/>
+      <c r="J4" s="97"/>
+      <c r="K4" s="98"/>
+    </row>
+    <row r="5" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="113"/>
+      <c r="B5" s="113"/>
+      <c r="C5" s="113"/>
+      <c r="D5" s="113"/>
+      <c r="E5" s="113"/>
+      <c r="F5" s="113"/>
+      <c r="G5" s="113"/>
+      <c r="H5" s="113"/>
+      <c r="I5" s="113"/>
+      <c r="J5" s="113"/>
+      <c r="K5" s="113"/>
+    </row>
+    <row r="6" spans="1:11" s="19" customFormat="1" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="95" t="s">
+      <c r="B6" s="114" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="95"/>
+      <c r="C6" s="114"/>
       <c r="D6" s="23" t="s">
         <v>8</v>
       </c>
@@ -2405,15 +2420,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="64">
         <v>1</v>
       </c>
-      <c r="B7" s="115" t="str">
+      <c r="B7" s="106" t="str">
         <f>C2</f>
         <v>Zerhuel Bussiness Networking</v>
       </c>
-      <c r="C7" s="116"/>
+      <c r="C7" s="107"/>
       <c r="D7" s="46"/>
       <c r="E7" s="46"/>
       <c r="F7" s="66"/>
@@ -2423,14 +2438,14 @@
       <c r="J7" s="46"/>
       <c r="K7" s="58"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="44">
         <v>2</v>
       </c>
-      <c r="B8" s="85" t="s">
+      <c r="B8" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="86"/>
+      <c r="C8" s="90"/>
       <c r="D8" s="48"/>
       <c r="E8" s="48"/>
       <c r="F8" s="67"/>
@@ -2440,14 +2455,14 @@
       <c r="J8" s="48"/>
       <c r="K8" s="59"/>
     </row>
-    <row r="9" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="44">
         <v>3</v>
       </c>
-      <c r="B9" s="83" t="s">
+      <c r="B9" s="85" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="84"/>
+      <c r="C9" s="86"/>
       <c r="D9" s="35"/>
       <c r="E9" s="35" t="s">
         <v>29</v>
@@ -2469,14 +2484,14 @@
         <v>95</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="33" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" s="33" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="44">
         <v>4</v>
       </c>
-      <c r="B10" s="83" t="s">
+      <c r="B10" s="85" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="84"/>
+      <c r="C10" s="86"/>
       <c r="D10" s="37"/>
       <c r="E10" s="35" t="s">
         <v>29</v>
@@ -2498,14 +2513,14 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="34">
         <v>5</v>
       </c>
-      <c r="B11" s="83" t="s">
+      <c r="B11" s="85" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="84"/>
+      <c r="C11" s="86"/>
       <c r="D11" s="39"/>
       <c r="E11" s="35" t="s">
         <v>29</v>
@@ -2527,14 +2542,14 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="44">
         <v>8</v>
       </c>
-      <c r="B12" s="83" t="s">
+      <c r="B12" s="85" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="84"/>
+      <c r="C12" s="86"/>
       <c r="D12" s="35"/>
       <c r="E12" s="35" t="s">
         <v>28</v>
@@ -2556,10 +2571,10 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="44"/>
-      <c r="B13" s="83"/>
-      <c r="C13" s="84"/>
+      <c r="B13" s="85"/>
+      <c r="C13" s="86"/>
       <c r="D13" s="35"/>
       <c r="E13" s="35"/>
       <c r="F13" s="68"/>
@@ -2569,14 +2584,14 @@
       <c r="J13" s="35"/>
       <c r="K13" s="26"/>
     </row>
-    <row r="14" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="44">
         <v>9</v>
       </c>
-      <c r="B14" s="85" t="s">
+      <c r="B14" s="89" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="86"/>
+      <c r="C14" s="90"/>
       <c r="D14" s="48"/>
       <c r="E14" s="48"/>
       <c r="F14" s="67"/>
@@ -2586,14 +2601,14 @@
       <c r="J14" s="48"/>
       <c r="K14" s="59"/>
     </row>
-    <row r="15" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="44">
         <v>10</v>
       </c>
-      <c r="B15" s="83" t="s">
+      <c r="B15" s="85" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="84"/>
+      <c r="C15" s="86"/>
       <c r="D15" s="35"/>
       <c r="E15" s="35" t="s">
         <v>29</v>
@@ -2615,14 +2630,14 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="44">
         <v>11</v>
       </c>
-      <c r="B16" s="83" t="s">
+      <c r="B16" s="85" t="s">
         <v>64</v>
       </c>
-      <c r="C16" s="84"/>
+      <c r="C16" s="86"/>
       <c r="D16" s="35"/>
       <c r="E16" s="35" t="s">
         <v>29</v>
@@ -2644,14 +2659,14 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="44">
         <v>12</v>
       </c>
-      <c r="B17" s="110" t="s">
+      <c r="B17" s="99" t="s">
         <v>65</v>
       </c>
-      <c r="C17" s="111"/>
+      <c r="C17" s="100"/>
       <c r="D17" s="73"/>
       <c r="E17" s="35" t="s">
         <v>28</v>
@@ -2673,14 +2688,14 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="44">
         <v>13</v>
       </c>
-      <c r="B18" s="83" t="s">
+      <c r="B18" s="85" t="s">
         <v>66</v>
       </c>
-      <c r="C18" s="84"/>
+      <c r="C18" s="86"/>
       <c r="D18" s="35"/>
       <c r="E18" s="35" t="s">
         <v>28</v>
@@ -2700,14 +2715,14 @@
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="44">
         <v>14</v>
       </c>
-      <c r="B19" s="83" t="s">
+      <c r="B19" s="85" t="s">
         <v>87</v>
       </c>
-      <c r="C19" s="84"/>
+      <c r="C19" s="86"/>
       <c r="D19" s="35"/>
       <c r="E19" s="35" t="s">
         <v>29</v>
@@ -2729,14 +2744,14 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="44">
         <v>15</v>
       </c>
-      <c r="B20" s="83" t="s">
+      <c r="B20" s="85" t="s">
         <v>67</v>
       </c>
-      <c r="C20" s="84"/>
+      <c r="C20" s="86"/>
       <c r="D20" s="35"/>
       <c r="E20" s="35" t="s">
         <v>28</v>
@@ -2756,14 +2771,14 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="44">
         <v>16</v>
       </c>
-      <c r="B21" s="83" t="s">
+      <c r="B21" s="85" t="s">
         <v>68</v>
       </c>
-      <c r="C21" s="84"/>
+      <c r="C21" s="86"/>
       <c r="D21" s="35"/>
       <c r="E21" s="35" t="s">
         <v>29</v>
@@ -2785,14 +2800,14 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="44">
         <v>17</v>
       </c>
-      <c r="B22" s="83" t="s">
+      <c r="B22" s="85" t="s">
         <v>69</v>
       </c>
-      <c r="C22" s="84"/>
+      <c r="C22" s="86"/>
       <c r="D22" s="35"/>
       <c r="E22" s="35" t="s">
         <v>29</v>
@@ -2814,14 +2829,14 @@
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="44">
         <v>18</v>
       </c>
-      <c r="B23" s="83" t="s">
+      <c r="B23" s="85" t="s">
         <v>70</v>
       </c>
-      <c r="C23" s="84"/>
+      <c r="C23" s="86"/>
       <c r="D23" s="35"/>
       <c r="E23" s="35" t="s">
         <v>28</v>
@@ -2841,14 +2856,14 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="44">
         <v>19</v>
       </c>
-      <c r="B24" s="83" t="s">
+      <c r="B24" s="85" t="s">
         <v>71</v>
       </c>
-      <c r="C24" s="84"/>
+      <c r="C24" s="86"/>
       <c r="D24" s="35"/>
       <c r="E24" s="35" t="s">
         <v>29</v>
@@ -2870,10 +2885,10 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="44"/>
-      <c r="B25" s="83"/>
-      <c r="C25" s="84"/>
+      <c r="B25" s="85"/>
+      <c r="C25" s="86"/>
       <c r="D25" s="35"/>
       <c r="E25" s="35"/>
       <c r="F25" s="68"/>
@@ -2883,10 +2898,10 @@
       <c r="J25" s="35"/>
       <c r="K25" s="26"/>
     </row>
-    <row r="26" spans="1:11" s="33" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" s="33" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="44"/>
-      <c r="B26" s="118"/>
-      <c r="C26" s="119"/>
+      <c r="B26" s="95"/>
+      <c r="C26" s="96"/>
       <c r="D26" s="37"/>
       <c r="E26" s="35"/>
       <c r="F26" s="68"/>
@@ -2896,14 +2911,14 @@
       <c r="J26" s="37"/>
       <c r="K26" s="26"/>
     </row>
-    <row r="27" spans="1:11" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="34">
         <v>21</v>
       </c>
-      <c r="B27" s="85" t="s">
+      <c r="B27" s="89" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="86"/>
+      <c r="C27" s="90"/>
       <c r="D27" s="52"/>
       <c r="E27" s="52"/>
       <c r="F27" s="70"/>
@@ -2913,14 +2928,14 @@
       <c r="J27" s="52"/>
       <c r="K27" s="61"/>
     </row>
-    <row r="28" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="44">
         <v>22</v>
       </c>
-      <c r="B28" s="83" t="s">
+      <c r="B28" s="85" t="s">
         <v>90</v>
       </c>
-      <c r="C28" s="84"/>
+      <c r="C28" s="86"/>
       <c r="D28" s="35"/>
       <c r="E28" s="35" t="s">
         <v>29</v>
@@ -2940,14 +2955,14 @@
         <v>95</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="34">
         <v>23</v>
       </c>
-      <c r="B29" s="83" t="s">
+      <c r="B29" s="85" t="s">
         <v>72</v>
       </c>
-      <c r="C29" s="84"/>
+      <c r="C29" s="86"/>
       <c r="D29" s="35"/>
       <c r="E29" s="35" t="s">
         <v>28</v>
@@ -2967,14 +2982,14 @@
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="44">
         <v>24</v>
       </c>
-      <c r="B30" s="83" t="s">
+      <c r="B30" s="85" t="s">
         <v>73</v>
       </c>
-      <c r="C30" s="84"/>
+      <c r="C30" s="86"/>
       <c r="D30" s="35"/>
       <c r="E30" s="35" t="s">
         <v>28</v>
@@ -2994,14 +3009,14 @@
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="34">
         <v>25</v>
       </c>
-      <c r="B31" s="83" t="s">
+      <c r="B31" s="85" t="s">
         <v>74</v>
       </c>
-      <c r="C31" s="84"/>
+      <c r="C31" s="86"/>
       <c r="D31" s="35"/>
       <c r="E31" s="35" t="s">
         <v>28</v>
@@ -3021,14 +3036,14 @@
         <v>95</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="44">
         <v>26</v>
       </c>
-      <c r="B32" s="83" t="s">
+      <c r="B32" s="85" t="s">
         <v>75</v>
       </c>
-      <c r="C32" s="84"/>
+      <c r="C32" s="86"/>
       <c r="D32" s="35"/>
       <c r="E32" s="35" t="s">
         <v>28</v>
@@ -3048,14 +3063,14 @@
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="34">
         <v>27</v>
       </c>
-      <c r="B33" s="83" t="s">
+      <c r="B33" s="85" t="s">
         <v>77</v>
       </c>
-      <c r="C33" s="84"/>
+      <c r="C33" s="86"/>
       <c r="D33" s="35"/>
       <c r="E33" s="35" t="s">
         <v>28</v>
@@ -3075,12 +3090,12 @@
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="34"/>
-      <c r="B34" s="83" t="s">
+      <c r="B34" s="85" t="s">
         <v>76</v>
       </c>
-      <c r="C34" s="84"/>
+      <c r="C34" s="86"/>
       <c r="D34" s="35"/>
       <c r="E34" s="35" t="s">
         <v>28</v>
@@ -3100,12 +3115,12 @@
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="34"/>
-      <c r="B35" s="83" t="s">
+      <c r="B35" s="85" t="s">
         <v>78</v>
       </c>
-      <c r="C35" s="84"/>
+      <c r="C35" s="86"/>
       <c r="D35" s="35"/>
       <c r="E35" s="35" t="s">
         <v>28</v>
@@ -3125,12 +3140,12 @@
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="34"/>
-      <c r="B36" s="83" t="s">
+      <c r="B36" s="85" t="s">
         <v>79</v>
       </c>
-      <c r="C36" s="84"/>
+      <c r="C36" s="86"/>
       <c r="D36" s="35"/>
       <c r="E36" s="35" t="s">
         <v>28</v>
@@ -3150,12 +3165,12 @@
         <v>95</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="34"/>
-      <c r="B37" s="83" t="s">
+      <c r="B37" s="85" t="s">
         <v>80</v>
       </c>
-      <c r="C37" s="84"/>
+      <c r="C37" s="86"/>
       <c r="D37" s="35"/>
       <c r="E37" s="35" t="s">
         <v>28</v>
@@ -3175,12 +3190,12 @@
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="34"/>
-      <c r="B38" s="83" t="s">
+      <c r="B38" s="85" t="s">
         <v>81</v>
       </c>
-      <c r="C38" s="84"/>
+      <c r="C38" s="86"/>
       <c r="D38" s="35"/>
       <c r="E38" s="35" t="s">
         <v>28</v>
@@ -3200,12 +3215,12 @@
         <v>95</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="34"/>
-      <c r="B39" s="83" t="s">
+      <c r="B39" s="85" t="s">
         <v>84</v>
       </c>
-      <c r="C39" s="84"/>
+      <c r="C39" s="86"/>
       <c r="D39" s="35"/>
       <c r="E39" s="35" t="s">
         <v>28</v>
@@ -3225,12 +3240,12 @@
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="34"/>
-      <c r="B40" s="83" t="s">
+      <c r="B40" s="85" t="s">
         <v>82</v>
       </c>
-      <c r="C40" s="84"/>
+      <c r="C40" s="86"/>
       <c r="D40" s="35"/>
       <c r="E40" s="35" t="s">
         <v>28</v>
@@ -3250,12 +3265,12 @@
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="34"/>
-      <c r="B41" s="83" t="s">
+      <c r="B41" s="85" t="s">
         <v>83</v>
       </c>
-      <c r="C41" s="84"/>
+      <c r="C41" s="86"/>
       <c r="D41" s="35"/>
       <c r="E41" s="35" t="s">
         <v>28</v>
@@ -3275,12 +3290,12 @@
         <v>95</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="34"/>
-      <c r="B42" s="83" t="s">
+      <c r="B42" s="85" t="s">
         <v>85</v>
       </c>
-      <c r="C42" s="84"/>
+      <c r="C42" s="86"/>
       <c r="D42" s="35"/>
       <c r="E42" s="35" t="s">
         <v>28</v>
@@ -3300,10 +3315,10 @@
         <v>95</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="44"/>
-      <c r="B43" s="121"/>
-      <c r="C43" s="122"/>
+      <c r="B43" s="87"/>
+      <c r="C43" s="88"/>
       <c r="D43" s="35"/>
       <c r="E43" s="35"/>
       <c r="F43" s="68"/>
@@ -3313,14 +3328,14 @@
       <c r="J43" s="35"/>
       <c r="K43" s="26"/>
     </row>
-    <row r="44" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="44">
         <v>28</v>
       </c>
-      <c r="B44" s="85" t="s">
+      <c r="B44" s="89" t="s">
         <v>19</v>
       </c>
-      <c r="C44" s="86"/>
+      <c r="C44" s="90"/>
       <c r="D44" s="48"/>
       <c r="E44" s="48"/>
       <c r="F44" s="67"/>
@@ -3330,14 +3345,14 @@
       <c r="J44" s="48"/>
       <c r="K44" s="59"/>
     </row>
-    <row r="45" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="44">
         <v>29</v>
       </c>
-      <c r="B45" s="83" t="s">
+      <c r="B45" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="C45" s="84"/>
+      <c r="C45" s="86"/>
       <c r="D45" s="35"/>
       <c r="E45" s="35" t="s">
         <v>28</v>
@@ -3357,14 +3372,14 @@
         <v>62</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="44">
         <v>30</v>
       </c>
-      <c r="B46" s="83" t="s">
+      <c r="B46" s="85" t="s">
         <v>56</v>
       </c>
-      <c r="C46" s="84"/>
+      <c r="C46" s="86"/>
       <c r="D46" s="35"/>
       <c r="E46" s="35" t="s">
         <v>28</v>
@@ -3384,10 +3399,10 @@
         <v>95</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="44"/>
-      <c r="B47" s="83"/>
-      <c r="C47" s="84"/>
+      <c r="B47" s="85"/>
+      <c r="C47" s="86"/>
       <c r="D47" s="35"/>
       <c r="E47" s="35"/>
       <c r="F47" s="68"/>
@@ -3397,14 +3412,14 @@
       <c r="J47" s="35"/>
       <c r="K47" s="26"/>
     </row>
-    <row r="48" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="44">
         <v>31</v>
       </c>
-      <c r="B48" s="85" t="s">
+      <c r="B48" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="C48" s="86"/>
+      <c r="C48" s="90"/>
       <c r="D48" s="48"/>
       <c r="E48" s="48"/>
       <c r="F48" s="67"/>
@@ -3414,14 +3429,14 @@
       <c r="J48" s="48"/>
       <c r="K48" s="59"/>
     </row>
-    <row r="49" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="44">
         <v>32</v>
       </c>
-      <c r="B49" s="83" t="s">
+      <c r="B49" s="85" t="s">
         <v>55</v>
       </c>
-      <c r="C49" s="84"/>
+      <c r="C49" s="86"/>
       <c r="D49" s="35"/>
       <c r="E49" s="35" t="s">
         <v>28</v>
@@ -3441,10 +3456,10 @@
         <v>96</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="29"/>
-      <c r="B50" s="83"/>
-      <c r="C50" s="84"/>
+      <c r="B50" s="85"/>
+      <c r="C50" s="86"/>
       <c r="D50" s="41"/>
       <c r="E50" s="35"/>
       <c r="F50" s="71"/>
@@ -3454,14 +3469,14 @@
       <c r="J50" s="41"/>
       <c r="K50" s="62"/>
     </row>
-    <row r="51" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="44">
         <v>33</v>
       </c>
-      <c r="B51" s="85" t="s">
+      <c r="B51" s="89" t="s">
         <v>22</v>
       </c>
-      <c r="C51" s="86"/>
+      <c r="C51" s="90"/>
       <c r="D51" s="48"/>
       <c r="E51" s="48"/>
       <c r="F51" s="67"/>
@@ -3471,14 +3486,14 @@
       <c r="J51" s="48"/>
       <c r="K51" s="59"/>
     </row>
-    <row r="52" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="44">
         <v>34</v>
       </c>
-      <c r="B52" s="83" t="s">
+      <c r="B52" s="85" t="s">
         <v>23</v>
       </c>
-      <c r="C52" s="84"/>
+      <c r="C52" s="86"/>
       <c r="D52" s="35"/>
       <c r="E52" s="35" t="s">
         <v>28</v>
@@ -3498,14 +3513,14 @@
         <v>61</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="44">
         <v>35</v>
       </c>
-      <c r="B53" s="83" t="s">
+      <c r="B53" s="85" t="s">
         <v>86</v>
       </c>
-      <c r="C53" s="84"/>
+      <c r="C53" s="86"/>
       <c r="D53" s="35"/>
       <c r="E53" s="35" t="s">
         <v>28</v>
@@ -3527,10 +3542,10 @@
         <v>61</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="44"/>
-      <c r="B54" s="83"/>
-      <c r="C54" s="84"/>
+      <c r="B54" s="85"/>
+      <c r="C54" s="86"/>
       <c r="D54" s="35"/>
       <c r="F54" s="68"/>
       <c r="G54" s="36"/>
@@ -3539,12 +3554,12 @@
       <c r="J54" s="35"/>
       <c r="K54" s="26"/>
     </row>
-    <row r="55" spans="1:11" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="65"/>
-      <c r="B55" s="87" t="s">
+      <c r="B55" s="125" t="s">
         <v>24</v>
       </c>
-      <c r="C55" s="88"/>
+      <c r="C55" s="126"/>
       <c r="D55" s="55"/>
       <c r="E55" s="55"/>
       <c r="F55" s="72"/>
@@ -3554,12 +3569,12 @@
       <c r="J55" s="55"/>
       <c r="K55" s="63"/>
     </row>
-    <row r="56" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="57" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="125" t="s">
+    <row r="56" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="57" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B57" s="93" t="s">
         <v>25</v>
       </c>
-      <c r="C57" s="126"/>
+      <c r="C57" s="94"/>
       <c r="D57" s="78"/>
       <c r="E57" s="78"/>
       <c r="F57" s="78" t="s">
@@ -3572,8 +3587,8 @@
       </c>
       <c r="K57"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B58" s="123" t="s">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B58" s="91" t="s">
         <v>9</v>
       </c>
       <c r="C58" s="76" t="s">
@@ -3587,8 +3602,8 @@
       <c r="I58" s="81"/>
       <c r="K58"/>
     </row>
-    <row r="59" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="124"/>
+    <row r="59" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B59" s="92"/>
       <c r="C59" s="77" t="s">
         <v>29</v>
       </c>
@@ -3600,7 +3615,7 @@
       <c r="I59" s="81"/>
       <c r="K59"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B60" s="78"/>
       <c r="C60" s="78"/>
       <c r="D60" s="78"/>
@@ -3615,7 +3630,7 @@
       </c>
       <c r="K60"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B61" s="78"/>
       <c r="C61" s="78"/>
       <c r="D61" s="78"/>
@@ -3630,48 +3645,100 @@
       </c>
       <c r="K61"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B62" s="78"/>
       <c r="C62" s="78"/>
       <c r="D62" s="78"/>
       <c r="E62" s="78"/>
-      <c r="F62" s="117"/>
-      <c r="G62" s="117"/>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F62" s="83"/>
+      <c r="G62" s="83"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B63" s="78"/>
       <c r="C63" s="78"/>
       <c r="D63" s="78"/>
       <c r="E63" s="78"/>
-      <c r="F63" s="117"/>
-      <c r="G63" s="117"/>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F63" s="83"/>
+      <c r="G63" s="83"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B64" s="78"/>
       <c r="C64" s="78"/>
       <c r="D64" s="78"/>
       <c r="E64" s="78"/>
-      <c r="F64" s="117"/>
-      <c r="G64" s="117"/>
-    </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F64" s="83"/>
+      <c r="G64" s="83"/>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B65" s="78"/>
       <c r="C65" s="79"/>
       <c r="D65" s="78"/>
       <c r="E65" s="78"/>
-      <c r="F65" s="120"/>
-      <c r="G65" s="120"/>
-    </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F65" s="84"/>
+      <c r="G65" s="84"/>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B66" s="78"/>
       <c r="C66" s="78"/>
       <c r="D66" s="78"/>
       <c r="E66" s="78"/>
-      <c r="F66" s="117"/>
-      <c r="G66" s="117"/>
+      <c r="F66" s="83"/>
+      <c r="G66" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="68">
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A5:K5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
     <mergeCell ref="F62:G62"/>
     <mergeCell ref="F63:G63"/>
     <mergeCell ref="F64:G64"/>
@@ -3688,58 +3755,6 @@
     <mergeCell ref="B57:C57"/>
     <mergeCell ref="B54:C54"/>
     <mergeCell ref="B49:C49"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A5:K5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="C2:G2"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7:E8 E14 E27 E44 E48 E51 E55">
@@ -3754,115 +3769,115 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O41"/>
+  <dimension ref="A1:S41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" style="25" customWidth="1"/>
-    <col min="2" max="2" width="37.42578125" customWidth="1"/>
-    <col min="3" max="5" width="3.7109375" customWidth="1"/>
-    <col min="6" max="6" width="3.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" customWidth="1"/>
-    <col min="8" max="8" width="21.85546875" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" style="25" customWidth="1"/>
+    <col min="2" max="2" width="37.44140625" customWidth="1"/>
+    <col min="3" max="5" width="3.6640625" customWidth="1"/>
+    <col min="6" max="6" width="3.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16.88671875" customWidth="1"/>
+    <col min="8" max="8" width="21.88671875" customWidth="1"/>
     <col min="9" max="9" width="20" customWidth="1"/>
-    <col min="10" max="10" width="31.42578125" customWidth="1"/>
+    <col min="10" max="10" width="31.44140625" customWidth="1"/>
     <col min="11" max="11" width="21" customWidth="1"/>
-    <col min="12" max="12" width="9.42578125" customWidth="1"/>
+    <col min="12" max="12" width="9.44140625" customWidth="1"/>
     <col min="13" max="13" width="7" customWidth="1"/>
-    <col min="14" max="15" width="8.5703125" customWidth="1"/>
+    <col min="14" max="15" width="8.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="89" t="s">
+    <row r="1" spans="1:19" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="108" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
-      <c r="H1" s="91"/>
-      <c r="I1" s="91"/>
-      <c r="J1" s="91"/>
-      <c r="K1" s="91"/>
-      <c r="L1" s="92"/>
-      <c r="M1" s="92"/>
-      <c r="N1" s="92"/>
-      <c r="O1" s="93"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="127" t="s">
+      <c r="B1" s="109"/>
+      <c r="C1" s="110"/>
+      <c r="D1" s="110"/>
+      <c r="E1" s="110"/>
+      <c r="F1" s="110"/>
+      <c r="G1" s="110"/>
+      <c r="H1" s="110"/>
+      <c r="I1" s="110"/>
+      <c r="J1" s="110"/>
+      <c r="K1" s="110"/>
+      <c r="L1" s="111"/>
+      <c r="M1" s="111"/>
+      <c r="N1" s="111"/>
+      <c r="O1" s="112"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" s="153" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="128"/>
-      <c r="C2" s="100" t="s">
+      <c r="B2" s="154"/>
+      <c r="C2" s="117" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="101"/>
-      <c r="E2" s="101"/>
-      <c r="F2" s="101"/>
-      <c r="G2" s="101"/>
-      <c r="H2" s="102"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="118"/>
+      <c r="F2" s="118"/>
+      <c r="G2" s="118"/>
+      <c r="H2" s="119"/>
       <c r="I2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="106" t="s">
+      <c r="J2" s="123" t="s">
         <v>57</v>
       </c>
-      <c r="K2" s="107"/>
-      <c r="L2" s="106"/>
-      <c r="M2" s="107"/>
-      <c r="N2" s="106"/>
-      <c r="O2" s="107"/>
-    </row>
-    <row r="3" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="129" t="s">
+      <c r="K2" s="124"/>
+      <c r="L2" s="123"/>
+      <c r="M2" s="124"/>
+      <c r="N2" s="123"/>
+      <c r="O2" s="124"/>
+    </row>
+    <row r="3" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="155" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="130"/>
-      <c r="C3" s="103" t="s">
+      <c r="B3" s="156"/>
+      <c r="C3" s="120" t="s">
         <v>94</v>
       </c>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="105"/>
+      <c r="D3" s="121"/>
+      <c r="E3" s="121"/>
+      <c r="F3" s="121"/>
+      <c r="G3" s="121"/>
+      <c r="H3" s="122"/>
       <c r="I3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="131">
+      <c r="J3" s="157">
         <v>43466</v>
       </c>
-      <c r="K3" s="108"/>
-      <c r="L3" s="108"/>
-      <c r="M3" s="108"/>
-      <c r="N3" s="108"/>
-      <c r="O3" s="109"/>
-    </row>
-    <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="94"/>
-      <c r="B4" s="94"/>
-      <c r="C4" s="94"/>
-      <c r="D4" s="94"/>
-      <c r="E4" s="94"/>
-      <c r="F4" s="94"/>
-      <c r="G4" s="94"/>
-      <c r="H4" s="94"/>
-      <c r="I4" s="94"/>
-      <c r="J4" s="94"/>
-      <c r="K4" s="94"/>
-      <c r="L4" s="94"/>
-      <c r="M4" s="94"/>
-      <c r="N4" s="94"/>
-      <c r="O4" s="94"/>
-    </row>
-    <row r="5" spans="1:15" ht="65.25" x14ac:dyDescent="0.25">
+      <c r="K3" s="97"/>
+      <c r="L3" s="97"/>
+      <c r="M3" s="97"/>
+      <c r="N3" s="97"/>
+      <c r="O3" s="98"/>
+    </row>
+    <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="113"/>
+      <c r="B4" s="113"/>
+      <c r="C4" s="113"/>
+      <c r="D4" s="113"/>
+      <c r="E4" s="113"/>
+      <c r="F4" s="113"/>
+      <c r="G4" s="113"/>
+      <c r="H4" s="113"/>
+      <c r="I4" s="113"/>
+      <c r="J4" s="113"/>
+      <c r="K4" s="113"/>
+      <c r="L4" s="113"/>
+      <c r="M4" s="113"/>
+      <c r="N4" s="113"/>
+      <c r="O4" s="113"/>
+    </row>
+    <row r="5" spans="1:19" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A5" s="32" t="s">
         <v>6</v>
       </c>
@@ -3908,8 +3923,11 @@
       <c r="O5" s="21" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="44">
         <v>2</v>
       </c>
@@ -3931,7 +3949,7 @@
       <c r="N6" s="3"/>
       <c r="O6" s="4"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="44">
         <v>3</v>
       </c>
@@ -3953,7 +3971,7 @@
       <c r="N7" s="3"/>
       <c r="O7" s="4"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="44">
         <v>4</v>
       </c>
@@ -3975,7 +3993,7 @@
       <c r="N8" s="3"/>
       <c r="O8" s="4"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="44">
         <v>5</v>
       </c>
@@ -3997,7 +4015,7 @@
       <c r="N9" s="3"/>
       <c r="O9" s="4"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="44">
         <v>6</v>
       </c>
@@ -4019,7 +4037,7 @@
       <c r="N10" s="3"/>
       <c r="O10" s="4"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="44">
         <v>7</v>
       </c>
@@ -4041,7 +4059,7 @@
       <c r="N11" s="3"/>
       <c r="O11" s="4"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="44">
         <v>8</v>
       </c>
@@ -4063,7 +4081,7 @@
       <c r="N12" s="3"/>
       <c r="O12" s="4"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="44">
         <v>9</v>
       </c>
@@ -4085,7 +4103,7 @@
       <c r="N13" s="3"/>
       <c r="O13" s="4"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="44">
         <v>10</v>
       </c>
@@ -4106,8 +4124,11 @@
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
       <c r="O14" s="4"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="44">
         <v>11</v>
       </c>
@@ -4128,8 +4149,11 @@
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
       <c r="O15" s="4"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="44">
         <v>12</v>
       </c>
@@ -4150,8 +4174,14 @@
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
       <c r="O16" s="4"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R16" t="s">
+        <v>100</v>
+      </c>
+      <c r="S16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="44">
         <v>13</v>
       </c>
@@ -4173,7 +4203,7 @@
       <c r="N17" s="3"/>
       <c r="O17" s="4"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="44">
         <v>14</v>
       </c>
@@ -4195,7 +4225,7 @@
       <c r="N18" s="3"/>
       <c r="O18" s="4"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="44">
         <v>15</v>
       </c>
@@ -4217,7 +4247,7 @@
       <c r="N19" s="3"/>
       <c r="O19" s="4"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="44">
         <v>16</v>
       </c>
@@ -4239,7 +4269,7 @@
       <c r="N20" s="3"/>
       <c r="O20" s="4"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="44">
         <v>17</v>
       </c>
@@ -4261,7 +4291,7 @@
       <c r="N21" s="3"/>
       <c r="O21" s="4"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="44">
         <v>18</v>
       </c>
@@ -4283,7 +4313,7 @@
       <c r="N22" s="3"/>
       <c r="O22" s="4"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="44">
         <v>19</v>
       </c>
@@ -4305,7 +4335,7 @@
       <c r="N23" s="3"/>
       <c r="O23" s="4"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="44">
         <v>20</v>
       </c>
@@ -4327,7 +4357,7 @@
       <c r="N24" s="3"/>
       <c r="O24" s="4"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="44">
         <v>21</v>
       </c>
@@ -4349,7 +4379,7 @@
       <c r="N25" s="3"/>
       <c r="O25" s="4"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="44">
         <v>22</v>
       </c>
@@ -4371,7 +4401,7 @@
       <c r="N26" s="3"/>
       <c r="O26" s="4"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="44">
         <v>23</v>
       </c>
@@ -4393,7 +4423,7 @@
       <c r="N27" s="3"/>
       <c r="O27" s="4"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="44">
         <v>24</v>
       </c>
@@ -4415,7 +4445,7 @@
       <c r="N28" s="3"/>
       <c r="O28" s="4"/>
     </row>
-    <row r="29" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="24">
         <v>25</v>
       </c>
@@ -4437,122 +4467,131 @@
       <c r="N29" s="9"/>
       <c r="O29" s="5"/>
     </row>
-    <row r="31" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>46</v>
       </c>
       <c r="F31" s="43"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B32" s="138" t="s">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B32" s="133" t="s">
         <v>47</v>
       </c>
-      <c r="C32" s="141">
+      <c r="C32" s="136">
         <v>4</v>
       </c>
-      <c r="D32" s="142"/>
-      <c r="E32" s="142"/>
-      <c r="F32" s="143"/>
+      <c r="D32" s="137"/>
+      <c r="E32" s="137"/>
+      <c r="F32" s="138"/>
       <c r="G32" s="13"/>
       <c r="H32" s="13"/>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="139"/>
-      <c r="C33" s="144">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B33" s="134"/>
+      <c r="C33" s="139">
         <v>3</v>
       </c>
-      <c r="D33" s="145"/>
-      <c r="E33" s="145"/>
-      <c r="F33" s="146"/>
+      <c r="D33" s="140"/>
+      <c r="E33" s="140"/>
+      <c r="F33" s="141"/>
       <c r="G33" s="15"/>
       <c r="H33" s="15"/>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="139"/>
-      <c r="C34" s="144">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B34" s="134"/>
+      <c r="C34" s="139">
         <v>2</v>
       </c>
-      <c r="D34" s="145"/>
-      <c r="E34" s="145"/>
-      <c r="F34" s="146"/>
+      <c r="D34" s="140"/>
+      <c r="E34" s="140"/>
+      <c r="F34" s="141"/>
       <c r="G34" s="15"/>
       <c r="H34" s="15"/>
     </row>
-    <row r="35" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="140"/>
-      <c r="C35" s="147">
+    <row r="35" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B35" s="135"/>
+      <c r="C35" s="142">
         <v>1</v>
       </c>
-      <c r="D35" s="148"/>
-      <c r="E35" s="148"/>
-      <c r="F35" s="149"/>
+      <c r="D35" s="143"/>
+      <c r="E35" s="143"/>
+      <c r="F35" s="144"/>
       <c r="G35" s="15"/>
       <c r="H35" s="15"/>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="156" t="s">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B36" s="151" t="s">
         <v>38</v>
       </c>
-      <c r="C36" s="150" t="s">
+      <c r="C36" s="145" t="s">
         <v>48</v>
       </c>
-      <c r="D36" s="151"/>
-      <c r="E36" s="151"/>
-      <c r="F36" s="152"/>
+      <c r="D36" s="146"/>
+      <c r="E36" s="146"/>
+      <c r="F36" s="147"/>
       <c r="G36" s="15"/>
       <c r="H36" s="15"/>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="139"/>
-      <c r="C37" s="144" t="s">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B37" s="134"/>
+      <c r="C37" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="D37" s="145"/>
-      <c r="E37" s="145"/>
-      <c r="F37" s="146"/>
+      <c r="D37" s="140"/>
+      <c r="E37" s="140"/>
+      <c r="F37" s="141"/>
       <c r="G37" s="14"/>
       <c r="H37" s="14"/>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="139"/>
-      <c r="C38" s="144" t="s">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B38" s="134"/>
+      <c r="C38" s="139" t="s">
         <v>44</v>
       </c>
-      <c r="D38" s="145"/>
-      <c r="E38" s="145"/>
-      <c r="F38" s="146"/>
-    </row>
-    <row r="39" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="157"/>
-      <c r="C39" s="153" t="s">
+      <c r="D38" s="140"/>
+      <c r="E38" s="140"/>
+      <c r="F38" s="141"/>
+    </row>
+    <row r="39" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B39" s="152"/>
+      <c r="C39" s="148" t="s">
         <v>45</v>
       </c>
-      <c r="D39" s="154"/>
-      <c r="E39" s="154"/>
-      <c r="F39" s="155"/>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="136" t="s">
+      <c r="D39" s="149"/>
+      <c r="E39" s="149"/>
+      <c r="F39" s="150"/>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B40" s="131" t="s">
         <v>9</v>
       </c>
-      <c r="C40" s="132" t="s">
+      <c r="C40" s="127" t="s">
         <v>28</v>
       </c>
-      <c r="D40" s="132"/>
-      <c r="E40" s="132"/>
-      <c r="F40" s="133"/>
-    </row>
-    <row r="41" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="137"/>
-      <c r="C41" s="134" t="s">
+      <c r="D40" s="127"/>
+      <c r="E40" s="127"/>
+      <c r="F40" s="128"/>
+    </row>
+    <row r="41" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B41" s="132"/>
+      <c r="C41" s="129" t="s">
         <v>29</v>
       </c>
-      <c r="D41" s="134"/>
-      <c r="E41" s="134"/>
-      <c r="F41" s="135"/>
+      <c r="D41" s="129"/>
+      <c r="E41" s="129"/>
+      <c r="F41" s="130"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A4:O4"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="J3:O3"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:O2"/>
     <mergeCell ref="C40:F40"/>
     <mergeCell ref="C41:F41"/>
     <mergeCell ref="B40:B41"/>
@@ -4567,15 +4606,6 @@
     <mergeCell ref="C38:F38"/>
     <mergeCell ref="C39:F39"/>
     <mergeCell ref="B36:B39"/>
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="A4:O4"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="J3:O3"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="N2:O2"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14:E29">
@@ -4598,12 +4628,33 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Cost_x0020_Center xmlns="de1f3527-ee65-4171-8e88-278d1cad4dba" xsi:nil="true"/>
+    <SharedWithUsers xmlns="93e0a51c-8a94-4846-800d-92cf8a641c81">
+      <UserInfo>
+        <DisplayName>Mileesa Lumanog</DisplayName>
+        <AccountId>209</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Rosemarie Cris Flores</DisplayName>
+        <AccountId>207</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Malou Joy E. Bangcong</DisplayName>
+        <AccountId>273</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Leilah King</DisplayName>
+        <AccountId>208</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4815,39 +4866,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Cost_x0020_Center xmlns="de1f3527-ee65-4171-8e88-278d1cad4dba" xsi:nil="true"/>
-    <SharedWithUsers xmlns="93e0a51c-8a94-4846-800d-92cf8a641c81">
-      <UserInfo>
-        <DisplayName>Mileesa Lumanog</DisplayName>
-        <AccountId>209</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Rosemarie Cris Flores</DisplayName>
-        <AccountId>207</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Malou Joy E. Bangcong</DisplayName>
-        <AccountId>273</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Leilah King</DisplayName>
-        <AccountId>208</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{920A0596-903B-4E80-BD3E-00D8BD1A98DD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36FA0B68-4ACD-45C2-9A26-792212BEB904}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="de1f3527-ee65-4171-8e88-278d1cad4dba"/>
+    <ds:schemaRef ds:uri="93e0a51c-8a94-4846-800d-92cf8a641c81"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4873,12 +4906,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36FA0B68-4ACD-45C2-9A26-792212BEB904}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{920A0596-903B-4E80-BD3E-00D8BD1A98DD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="de1f3527-ee65-4171-8e88-278d1cad4dba"/>
-    <ds:schemaRef ds:uri="93e0a51c-8a94-4846-800d-92cf8a641c81"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>